<commit_message>
Implement option for limited Folder migration using Orchestrator 2020.4
</commit_message>
<xml_diff>
--- a/Workbooks/JA/フォルダー移行.xlsx
+++ b/Workbooks/JA/フォルダー移行.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateus.cruz\Documents\GitHub\OrchestratorManager\Workbooks\JA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0BBEA89-3344-4D9D-9CA4-A74776803C83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B5765B-779B-48F8-AACC-A9F7B9A0EC05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="プロセス" sheetId="4" r:id="rId1"/>
-    <sheet name="キュー" sheetId="8" r:id="rId2"/>
-    <sheet name="トリガー" sheetId="10" r:id="rId3"/>
-    <sheet name="ロボット" sheetId="11" r:id="rId4"/>
-    <sheet name="アセット" sheetId="7" r:id="rId5"/>
+    <sheet name="アセット" sheetId="12" r:id="rId2"/>
+    <sheet name="キュー" sheetId="8" r:id="rId3"/>
+    <sheet name="トリガー" sheetId="10" r:id="rId4"/>
+    <sheet name="ロボット" sheetId="11" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>クラッシックフォルダー名</t>
   </si>
@@ -57,9 +57,6 @@
     <t>アセット名</t>
   </si>
   <si>
-    <t>アセットの種類</t>
-  </si>
-  <si>
     <t>キュー名</t>
   </si>
   <si>
@@ -73,6 +70,12 @@
   </si>
   <si>
     <t>ロボットの移行ポリシー</t>
+  </si>
+  <si>
+    <t>アセットのスコープ</t>
+  </si>
+  <si>
+    <t>アセットの型</t>
   </si>
 </sst>
 </file>
@@ -221,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -249,158 +252,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="5"/>
-        </left>
-        <right style="thin">
-          <color theme="5"/>
-        </right>
-        <top style="thin">
-          <color theme="5"/>
-        </top>
-        <bottom style="thin">
-          <color theme="5"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
-        </bottom>
-      </border>
-      <protection locked="1" hidden="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFE7E6E6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="36">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -849,6 +722,203 @@
         </patternFill>
       </fill>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="5"/>
+        </right>
+        <top style="thin">
+          <color theme="5"/>
+        </top>
+        <bottom style="thin">
+          <color theme="5"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFE7E6E6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+      </border>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="5"/>
@@ -976,69 +1046,71 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:E201" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:E201" headerRowDxfId="35" dataDxfId="34">
   <autoFilter ref="A1:E201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="クラッシックフォルダー名" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{8B6D5F42-D711-499A-B47F-11E353F96F8A}" name="ロボットグループ名" dataDxfId="30"/>
-    <tableColumn id="1" xr3:uid="{585323CB-D400-49CC-B4C7-DE9E42C610A8}" name="プロセス名" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{13860EF0-E108-453A-B4F0-BF4407F583EB}" name="モダンフォルダー名" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{75FE23B7-3A10-47F6-A482-B742DB549888}" name="結果" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="クラッシックフォルダー名" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{8B6D5F42-D711-499A-B47F-11E353F96F8A}" name="ロボットグループ名" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{585323CB-D400-49CC-B4C7-DE9E42C610A8}" name="プロセス名" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{13860EF0-E108-453A-B4F0-BF4407F583EB}" name="モダンフォルダー名" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{75FE23B7-3A10-47F6-A482-B742DB549888}" name="結果" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00B4C8A0-1712-4F7A-B463-9C1FDDAFDCCD}" name="Table1467" displayName="Table1467" ref="A1:E201" headerRowDxfId="26" dataDxfId="25">
-  <autoFilter ref="A1:E201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="5">
-    <tableColumn id="4" xr3:uid="{0FCE192E-A981-480F-A92D-F8542A4EE432}" name="クラッシックフォルダー名" dataDxfId="24"/>
-    <tableColumn id="1" xr3:uid="{E17F75F7-594A-447B-ADC1-0DC311091523}" name="キュー名" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{38186110-EEFD-437A-8DF8-F98A919DE6E4}" name="キューの移行ポリシー" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{474FD516-64C7-4CC3-95F2-8B514943ED92}" name="モダンフォルダー名" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{05180D1D-9CF9-4061-A46F-E36171655A97}" name="結果" dataDxfId="20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{60ACC796-A34A-4192-89F2-15B992F41655}" name="Table1465" displayName="Table1465" ref="A1:G201" headerRowDxfId="28" dataDxfId="27">
+  <autoFilter ref="A1:G201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="7">
+    <tableColumn id="4" xr3:uid="{B71F2DE8-F8A0-4597-8303-3C62863AB8D8}" name="クラッシックフォルダー名" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{3AEC0C0D-C633-462D-93FD-0A8AB2BED01C}" name="アセット名" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{977E4B9B-1E2F-4E88-B938-F478A6D7D689}" name="アセットのスコープ" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{CC72ECDD-AE26-4908-9EBE-0EDD2CAE72F2}" name="ロボット名" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{00D7253E-5BF9-460B-B9AF-47D79CA1DE6A}" name="アセットの型" dataDxfId="22"/>
+    <tableColumn id="2" xr3:uid="{8F4A84CF-4B61-424D-88D3-1A3ED2AB483C}" name="モダンフォルダー名" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{4AAF5499-1343-453A-A366-6BA72B858BC6}" name="結果" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1B9C153C-F58A-4646-902F-75FEFCCA10CE}" name="Table1463" displayName="Table1463" ref="A1:D201" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A1:D201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="4">
-    <tableColumn id="4" xr3:uid="{6CBDCFE3-DD75-4BB2-B58F-78818266673E}" name="クラッシックフォルダー名" dataDxfId="17"/>
-    <tableColumn id="1" xr3:uid="{4296C484-DBA0-4BE4-9A5B-035A1DB1D1EB}" name="トリガー名" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{98C0D05B-9FE1-4790-B39D-924399DADA5A}" name="モダンフォルダー名" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{47054CF3-54B7-4C76-BD39-AF1C06C54D4E}" name="結果" dataDxfId="14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00B4C8A0-1712-4F7A-B463-9C1FDDAFDCCD}" name="Table1467" displayName="Table1467" ref="A1:E201" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A1:E201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="5">
+    <tableColumn id="4" xr3:uid="{0FCE192E-A981-480F-A92D-F8542A4EE432}" name="クラッシックフォルダー名" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{E17F75F7-594A-447B-ADC1-0DC311091523}" name="キュー名" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{38186110-EEFD-437A-8DF8-F98A919DE6E4}" name="キューの移行ポリシー" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{474FD516-64C7-4CC3-95F2-8B514943ED92}" name="モダンフォルダー名" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{05180D1D-9CF9-4061-A46F-E36171655A97}" name="結果" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{04A938D8-F1BB-4941-A012-2FDD12A7825F}" name="Table14672" displayName="Table14672" ref="A1:E201" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:E201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="5">
-    <tableColumn id="4" xr3:uid="{15C21256-243B-432D-BE72-873925151E77}" name="クラッシックフォルダー名" dataDxfId="11"/>
-    <tableColumn id="1" xr3:uid="{73F56336-6F99-4397-8380-780F84BB7E03}" name="ロボット名" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{A10EF349-36C9-45EF-A60B-F9767715C75A}" name="ロボットの移行ポリシー" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{0AB76F75-8D76-4749-8E35-0B76218834ED}" name="モダンフォルダー名" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{CAA02777-6A8D-480E-8B5F-9A633B17CA24}" name="結果" dataDxfId="7"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1B9C153C-F58A-4646-902F-75FEFCCA10CE}" name="Table1463" displayName="Table1463" ref="A1:D201" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:D201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="4">
+    <tableColumn id="4" xr3:uid="{6CBDCFE3-DD75-4BB2-B58F-78818266673E}" name="クラッシックフォルダー名" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{4296C484-DBA0-4BE4-9A5B-035A1DB1D1EB}" name="トリガー名" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{98C0D05B-9FE1-4790-B39D-924399DADA5A}" name="モダンフォルダー名" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{47054CF3-54B7-4C76-BD39-AF1C06C54D4E}" name="結果" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E855D032-1AF9-44A4-A76C-FA46D719AC02}" name="Table146" displayName="Table146" ref="A1:E201" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{04A938D8-F1BB-4941-A012-2FDD12A7825F}" name="Table14672" displayName="Table14672" ref="A1:E201" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A1:E201" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="5">
-    <tableColumn id="4" xr3:uid="{2F4E85AA-9073-4D99-B1CA-640FBC012059}" name="クラッシックフォルダー名" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{9086EF00-8740-408E-B6F1-645FF552018F}" name="アセット名" dataDxfId="3"/>
-    <tableColumn id="1" xr3:uid="{F32DDBA2-7A7E-4FBC-87DB-D1DF6EC8F25B}" name="アセットの種類" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{D0320155-A0E6-4CE0-B8D2-CEA0A58DB8F3}" name="モダンフォルダー名" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{8021FF53-C806-44D6-8817-531563561283}" name="結果" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{15C21256-243B-432D-BE72-873925151E77}" name="クラッシックフォルダー名" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{73F56336-6F99-4397-8380-780F84BB7E03}" name="ロボット名" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{A10EF349-36C9-45EF-A60B-F9767715C75A}" name="ロボットの移行ポリシー" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{0AB76F75-8D76-4749-8E35-0B76218834ED}" name="モダンフォルダー名" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{CAA02777-6A8D-480E-8B5F-9A633B17CA24}" name="結果" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2748,6 +2820,1867 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5A80C3E-71B9-4620-A62A-4A16297A1F9E}">
+  <dimension ref="A1:G201"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="7" customWidth="1"/>
+    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="45.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="13"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="13"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="13"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="13"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="13"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="13"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="13"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="13"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="13"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="13"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="13"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="13"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="13"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="13"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="13"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="13"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="13"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="13"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="13"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="13"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="13"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="13"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="13"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="13"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="13"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="13"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="13"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="13"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="13"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="13"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="13"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="13"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="13"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="13"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="13"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="13"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="13"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="13"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="13"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="13"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="13"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="13"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="13"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="13"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="13"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="13"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="13"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="13"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="13"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="13"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="13"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="13"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="13"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="13"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="13"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="13"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="13"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="13"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="13"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="13"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="13"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="15"/>
+      <c r="G44" s="13"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="13"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="13"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="13"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="15"/>
+      <c r="G46" s="13"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="13"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="15"/>
+      <c r="G47" s="13"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="13"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="15"/>
+      <c r="G48" s="13"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="13"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="15"/>
+      <c r="G49" s="13"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="13"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="13"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="13"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="15"/>
+      <c r="G51" s="13"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="13"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="15"/>
+      <c r="G52" s="13"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="13"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="15"/>
+      <c r="G53" s="13"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="13"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="15"/>
+      <c r="G54" s="13"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="13"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="15"/>
+      <c r="G55" s="13"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="13"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="15"/>
+      <c r="G56" s="13"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="13"/>
+      <c r="B57" s="13"/>
+      <c r="C57" s="13"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="15"/>
+      <c r="G57" s="13"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="13"/>
+      <c r="B58" s="13"/>
+      <c r="C58" s="13"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="15"/>
+      <c r="G58" s="13"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="13"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="13"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="13"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="13"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="13"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="13"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="13"/>
+      <c r="B61" s="13"/>
+      <c r="C61" s="13"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="15"/>
+      <c r="G61" s="13"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="13"/>
+      <c r="B62" s="13"/>
+      <c r="C62" s="13"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="15"/>
+      <c r="G62" s="13"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="13"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="13"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="13"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="13"/>
+      <c r="B64" s="13"/>
+      <c r="C64" s="13"/>
+      <c r="D64" s="13"/>
+      <c r="E64" s="13"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="13"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="13"/>
+      <c r="B65" s="13"/>
+      <c r="C65" s="13"/>
+      <c r="D65" s="13"/>
+      <c r="E65" s="13"/>
+      <c r="F65" s="15"/>
+      <c r="G65" s="13"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="13"/>
+      <c r="B66" s="13"/>
+      <c r="C66" s="13"/>
+      <c r="D66" s="13"/>
+      <c r="E66" s="13"/>
+      <c r="F66" s="15"/>
+      <c r="G66" s="13"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="13"/>
+      <c r="B67" s="13"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="13"/>
+      <c r="E67" s="13"/>
+      <c r="F67" s="15"/>
+      <c r="G67" s="13"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="13"/>
+      <c r="B68" s="13"/>
+      <c r="C68" s="13"/>
+      <c r="D68" s="13"/>
+      <c r="E68" s="13"/>
+      <c r="F68" s="15"/>
+      <c r="G68" s="13"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="13"/>
+      <c r="B69" s="13"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="13"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="15"/>
+      <c r="G69" s="13"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="13"/>
+      <c r="B70" s="13"/>
+      <c r="C70" s="13"/>
+      <c r="D70" s="13"/>
+      <c r="E70" s="13"/>
+      <c r="F70" s="15"/>
+      <c r="G70" s="13"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="13"/>
+      <c r="B71" s="13"/>
+      <c r="C71" s="13"/>
+      <c r="D71" s="13"/>
+      <c r="E71" s="13"/>
+      <c r="F71" s="15"/>
+      <c r="G71" s="13"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="13"/>
+      <c r="B72" s="13"/>
+      <c r="C72" s="13"/>
+      <c r="D72" s="13"/>
+      <c r="E72" s="13"/>
+      <c r="F72" s="15"/>
+      <c r="G72" s="13"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="13"/>
+      <c r="B73" s="13"/>
+      <c r="C73" s="13"/>
+      <c r="D73" s="13"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="15"/>
+      <c r="G73" s="13"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="13"/>
+      <c r="B74" s="13"/>
+      <c r="C74" s="13"/>
+      <c r="D74" s="13"/>
+      <c r="E74" s="13"/>
+      <c r="F74" s="15"/>
+      <c r="G74" s="13"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="13"/>
+      <c r="B75" s="13"/>
+      <c r="C75" s="13"/>
+      <c r="D75" s="13"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="15"/>
+      <c r="G75" s="13"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="13"/>
+      <c r="B76" s="13"/>
+      <c r="C76" s="13"/>
+      <c r="D76" s="13"/>
+      <c r="E76" s="13"/>
+      <c r="F76" s="15"/>
+      <c r="G76" s="13"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="13"/>
+      <c r="B77" s="13"/>
+      <c r="C77" s="13"/>
+      <c r="D77" s="13"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="15"/>
+      <c r="G77" s="13"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="13"/>
+      <c r="B78" s="13"/>
+      <c r="C78" s="13"/>
+      <c r="D78" s="13"/>
+      <c r="E78" s="13"/>
+      <c r="F78" s="15"/>
+      <c r="G78" s="13"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="13"/>
+      <c r="B79" s="13"/>
+      <c r="C79" s="13"/>
+      <c r="D79" s="13"/>
+      <c r="E79" s="13"/>
+      <c r="F79" s="15"/>
+      <c r="G79" s="13"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="13"/>
+      <c r="B80" s="13"/>
+      <c r="C80" s="13"/>
+      <c r="D80" s="13"/>
+      <c r="E80" s="13"/>
+      <c r="F80" s="15"/>
+      <c r="G80" s="13"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="13"/>
+      <c r="B81" s="13"/>
+      <c r="C81" s="13"/>
+      <c r="D81" s="13"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="15"/>
+      <c r="G81" s="13"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="13"/>
+      <c r="B82" s="13"/>
+      <c r="C82" s="13"/>
+      <c r="D82" s="13"/>
+      <c r="E82" s="13"/>
+      <c r="F82" s="15"/>
+      <c r="G82" s="13"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="13"/>
+      <c r="B83" s="13"/>
+      <c r="C83" s="13"/>
+      <c r="D83" s="13"/>
+      <c r="E83" s="13"/>
+      <c r="F83" s="15"/>
+      <c r="G83" s="13"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="13"/>
+      <c r="B84" s="13"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
+      <c r="E84" s="13"/>
+      <c r="F84" s="15"/>
+      <c r="G84" s="13"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="13"/>
+      <c r="B85" s="13"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="13"/>
+      <c r="E85" s="13"/>
+      <c r="F85" s="15"/>
+      <c r="G85" s="13"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="13"/>
+      <c r="B86" s="13"/>
+      <c r="C86" s="13"/>
+      <c r="D86" s="13"/>
+      <c r="E86" s="13"/>
+      <c r="F86" s="15"/>
+      <c r="G86" s="13"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="13"/>
+      <c r="B87" s="13"/>
+      <c r="C87" s="13"/>
+      <c r="D87" s="13"/>
+      <c r="E87" s="13"/>
+      <c r="F87" s="15"/>
+      <c r="G87" s="13"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="13"/>
+      <c r="B88" s="13"/>
+      <c r="C88" s="13"/>
+      <c r="D88" s="13"/>
+      <c r="E88" s="13"/>
+      <c r="F88" s="15"/>
+      <c r="G88" s="13"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="13"/>
+      <c r="B89" s="13"/>
+      <c r="C89" s="13"/>
+      <c r="D89" s="13"/>
+      <c r="E89" s="13"/>
+      <c r="F89" s="15"/>
+      <c r="G89" s="13"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="13"/>
+      <c r="B90" s="13"/>
+      <c r="C90" s="13"/>
+      <c r="D90" s="13"/>
+      <c r="E90" s="13"/>
+      <c r="F90" s="15"/>
+      <c r="G90" s="13"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="13"/>
+      <c r="B91" s="13"/>
+      <c r="C91" s="13"/>
+      <c r="D91" s="13"/>
+      <c r="E91" s="13"/>
+      <c r="F91" s="15"/>
+      <c r="G91" s="13"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="13"/>
+      <c r="B92" s="13"/>
+      <c r="C92" s="13"/>
+      <c r="D92" s="13"/>
+      <c r="E92" s="13"/>
+      <c r="F92" s="15"/>
+      <c r="G92" s="13"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="13"/>
+      <c r="B93" s="13"/>
+      <c r="C93" s="13"/>
+      <c r="D93" s="13"/>
+      <c r="E93" s="13"/>
+      <c r="F93" s="15"/>
+      <c r="G93" s="13"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="13"/>
+      <c r="B94" s="13"/>
+      <c r="C94" s="13"/>
+      <c r="D94" s="13"/>
+      <c r="E94" s="13"/>
+      <c r="F94" s="15"/>
+      <c r="G94" s="13"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="13"/>
+      <c r="B95" s="13"/>
+      <c r="C95" s="13"/>
+      <c r="D95" s="13"/>
+      <c r="E95" s="13"/>
+      <c r="F95" s="15"/>
+      <c r="G95" s="13"/>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="13"/>
+      <c r="B96" s="13"/>
+      <c r="C96" s="13"/>
+      <c r="D96" s="13"/>
+      <c r="E96" s="13"/>
+      <c r="F96" s="15"/>
+      <c r="G96" s="13"/>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="13"/>
+      <c r="B97" s="13"/>
+      <c r="C97" s="13"/>
+      <c r="D97" s="13"/>
+      <c r="E97" s="13"/>
+      <c r="F97" s="15"/>
+      <c r="G97" s="13"/>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="13"/>
+      <c r="B98" s="13"/>
+      <c r="C98" s="13"/>
+      <c r="D98" s="13"/>
+      <c r="E98" s="13"/>
+      <c r="F98" s="15"/>
+      <c r="G98" s="13"/>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="13"/>
+      <c r="B99" s="13"/>
+      <c r="C99" s="13"/>
+      <c r="D99" s="13"/>
+      <c r="E99" s="13"/>
+      <c r="F99" s="15"/>
+      <c r="G99" s="13"/>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="13"/>
+      <c r="B100" s="13"/>
+      <c r="C100" s="13"/>
+      <c r="D100" s="13"/>
+      <c r="E100" s="13"/>
+      <c r="F100" s="15"/>
+      <c r="G100" s="13"/>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="13"/>
+      <c r="B101" s="13"/>
+      <c r="C101" s="13"/>
+      <c r="D101" s="13"/>
+      <c r="E101" s="13"/>
+      <c r="F101" s="15"/>
+      <c r="G101" s="13"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="13"/>
+      <c r="B102" s="13"/>
+      <c r="C102" s="13"/>
+      <c r="D102" s="13"/>
+      <c r="E102" s="13"/>
+      <c r="F102" s="15"/>
+      <c r="G102" s="13"/>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="13"/>
+      <c r="B103" s="13"/>
+      <c r="C103" s="13"/>
+      <c r="D103" s="13"/>
+      <c r="E103" s="13"/>
+      <c r="F103" s="15"/>
+      <c r="G103" s="13"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="13"/>
+      <c r="B104" s="13"/>
+      <c r="C104" s="13"/>
+      <c r="D104" s="13"/>
+      <c r="E104" s="13"/>
+      <c r="F104" s="15"/>
+      <c r="G104" s="13"/>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="13"/>
+      <c r="B105" s="13"/>
+      <c r="C105" s="13"/>
+      <c r="D105" s="13"/>
+      <c r="E105" s="13"/>
+      <c r="F105" s="15"/>
+      <c r="G105" s="13"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="13"/>
+      <c r="B106" s="13"/>
+      <c r="C106" s="13"/>
+      <c r="D106" s="13"/>
+      <c r="E106" s="13"/>
+      <c r="F106" s="15"/>
+      <c r="G106" s="13"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="13"/>
+      <c r="B107" s="13"/>
+      <c r="C107" s="13"/>
+      <c r="D107" s="13"/>
+      <c r="E107" s="13"/>
+      <c r="F107" s="15"/>
+      <c r="G107" s="13"/>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="13"/>
+      <c r="B108" s="13"/>
+      <c r="C108" s="13"/>
+      <c r="D108" s="13"/>
+      <c r="E108" s="13"/>
+      <c r="F108" s="15"/>
+      <c r="G108" s="13"/>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="13"/>
+      <c r="B109" s="13"/>
+      <c r="C109" s="13"/>
+      <c r="D109" s="13"/>
+      <c r="E109" s="13"/>
+      <c r="F109" s="15"/>
+      <c r="G109" s="13"/>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="13"/>
+      <c r="B110" s="13"/>
+      <c r="C110" s="13"/>
+      <c r="D110" s="13"/>
+      <c r="E110" s="13"/>
+      <c r="F110" s="15"/>
+      <c r="G110" s="13"/>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="13"/>
+      <c r="B111" s="13"/>
+      <c r="C111" s="13"/>
+      <c r="D111" s="13"/>
+      <c r="E111" s="13"/>
+      <c r="F111" s="15"/>
+      <c r="G111" s="13"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="13"/>
+      <c r="B112" s="13"/>
+      <c r="C112" s="13"/>
+      <c r="D112" s="13"/>
+      <c r="E112" s="13"/>
+      <c r="F112" s="15"/>
+      <c r="G112" s="13"/>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="13"/>
+      <c r="B113" s="13"/>
+      <c r="C113" s="13"/>
+      <c r="D113" s="13"/>
+      <c r="E113" s="13"/>
+      <c r="F113" s="15"/>
+      <c r="G113" s="13"/>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="13"/>
+      <c r="B114" s="13"/>
+      <c r="C114" s="13"/>
+      <c r="D114" s="13"/>
+      <c r="E114" s="13"/>
+      <c r="F114" s="15"/>
+      <c r="G114" s="13"/>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" s="13"/>
+      <c r="B115" s="13"/>
+      <c r="C115" s="13"/>
+      <c r="D115" s="13"/>
+      <c r="E115" s="13"/>
+      <c r="F115" s="15"/>
+      <c r="G115" s="13"/>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="13"/>
+      <c r="B116" s="13"/>
+      <c r="C116" s="13"/>
+      <c r="D116" s="13"/>
+      <c r="E116" s="13"/>
+      <c r="F116" s="15"/>
+      <c r="G116" s="13"/>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="13"/>
+      <c r="B117" s="13"/>
+      <c r="C117" s="13"/>
+      <c r="D117" s="13"/>
+      <c r="E117" s="13"/>
+      <c r="F117" s="15"/>
+      <c r="G117" s="13"/>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="13"/>
+      <c r="B118" s="13"/>
+      <c r="C118" s="13"/>
+      <c r="D118" s="13"/>
+      <c r="E118" s="13"/>
+      <c r="F118" s="15"/>
+      <c r="G118" s="13"/>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="13"/>
+      <c r="B119" s="13"/>
+      <c r="C119" s="13"/>
+      <c r="D119" s="13"/>
+      <c r="E119" s="13"/>
+      <c r="F119" s="15"/>
+      <c r="G119" s="13"/>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" s="13"/>
+      <c r="B120" s="13"/>
+      <c r="C120" s="13"/>
+      <c r="D120" s="13"/>
+      <c r="E120" s="13"/>
+      <c r="F120" s="15"/>
+      <c r="G120" s="13"/>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" s="13"/>
+      <c r="B121" s="13"/>
+      <c r="C121" s="13"/>
+      <c r="D121" s="13"/>
+      <c r="E121" s="13"/>
+      <c r="F121" s="15"/>
+      <c r="G121" s="13"/>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" s="13"/>
+      <c r="B122" s="13"/>
+      <c r="C122" s="13"/>
+      <c r="D122" s="13"/>
+      <c r="E122" s="13"/>
+      <c r="F122" s="15"/>
+      <c r="G122" s="13"/>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" s="13"/>
+      <c r="B123" s="13"/>
+      <c r="C123" s="13"/>
+      <c r="D123" s="13"/>
+      <c r="E123" s="13"/>
+      <c r="F123" s="15"/>
+      <c r="G123" s="13"/>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" s="13"/>
+      <c r="B124" s="13"/>
+      <c r="C124" s="13"/>
+      <c r="D124" s="13"/>
+      <c r="E124" s="13"/>
+      <c r="F124" s="15"/>
+      <c r="G124" s="13"/>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" s="13"/>
+      <c r="B125" s="13"/>
+      <c r="C125" s="13"/>
+      <c r="D125" s="13"/>
+      <c r="E125" s="13"/>
+      <c r="F125" s="15"/>
+      <c r="G125" s="13"/>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" s="13"/>
+      <c r="B126" s="13"/>
+      <c r="C126" s="13"/>
+      <c r="D126" s="13"/>
+      <c r="E126" s="13"/>
+      <c r="F126" s="15"/>
+      <c r="G126" s="13"/>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" s="13"/>
+      <c r="B127" s="13"/>
+      <c r="C127" s="13"/>
+      <c r="D127" s="13"/>
+      <c r="E127" s="13"/>
+      <c r="F127" s="15"/>
+      <c r="G127" s="13"/>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" s="13"/>
+      <c r="B128" s="13"/>
+      <c r="C128" s="13"/>
+      <c r="D128" s="13"/>
+      <c r="E128" s="13"/>
+      <c r="F128" s="15"/>
+      <c r="G128" s="13"/>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129" s="13"/>
+      <c r="B129" s="13"/>
+      <c r="C129" s="13"/>
+      <c r="D129" s="13"/>
+      <c r="E129" s="13"/>
+      <c r="F129" s="15"/>
+      <c r="G129" s="13"/>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130" s="13"/>
+      <c r="B130" s="13"/>
+      <c r="C130" s="13"/>
+      <c r="D130" s="13"/>
+      <c r="E130" s="13"/>
+      <c r="F130" s="15"/>
+      <c r="G130" s="13"/>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131" s="13"/>
+      <c r="B131" s="13"/>
+      <c r="C131" s="13"/>
+      <c r="D131" s="13"/>
+      <c r="E131" s="13"/>
+      <c r="F131" s="15"/>
+      <c r="G131" s="13"/>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132" s="13"/>
+      <c r="B132" s="13"/>
+      <c r="C132" s="13"/>
+      <c r="D132" s="13"/>
+      <c r="E132" s="13"/>
+      <c r="F132" s="15"/>
+      <c r="G132" s="13"/>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133" s="13"/>
+      <c r="B133" s="13"/>
+      <c r="C133" s="13"/>
+      <c r="D133" s="13"/>
+      <c r="E133" s="13"/>
+      <c r="F133" s="15"/>
+      <c r="G133" s="13"/>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134" s="13"/>
+      <c r="B134" s="13"/>
+      <c r="C134" s="13"/>
+      <c r="D134" s="13"/>
+      <c r="E134" s="13"/>
+      <c r="F134" s="15"/>
+      <c r="G134" s="13"/>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135" s="13"/>
+      <c r="B135" s="13"/>
+      <c r="C135" s="13"/>
+      <c r="D135" s="13"/>
+      <c r="E135" s="13"/>
+      <c r="F135" s="15"/>
+      <c r="G135" s="13"/>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" s="13"/>
+      <c r="B136" s="13"/>
+      <c r="C136" s="13"/>
+      <c r="D136" s="13"/>
+      <c r="E136" s="13"/>
+      <c r="F136" s="15"/>
+      <c r="G136" s="13"/>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" s="13"/>
+      <c r="B137" s="13"/>
+      <c r="C137" s="13"/>
+      <c r="D137" s="13"/>
+      <c r="E137" s="13"/>
+      <c r="F137" s="15"/>
+      <c r="G137" s="13"/>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" s="13"/>
+      <c r="B138" s="13"/>
+      <c r="C138" s="13"/>
+      <c r="D138" s="13"/>
+      <c r="E138" s="13"/>
+      <c r="F138" s="15"/>
+      <c r="G138" s="13"/>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139" s="13"/>
+      <c r="B139" s="13"/>
+      <c r="C139" s="13"/>
+      <c r="D139" s="13"/>
+      <c r="E139" s="13"/>
+      <c r="F139" s="15"/>
+      <c r="G139" s="13"/>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140" s="13"/>
+      <c r="B140" s="13"/>
+      <c r="C140" s="13"/>
+      <c r="D140" s="13"/>
+      <c r="E140" s="13"/>
+      <c r="F140" s="15"/>
+      <c r="G140" s="13"/>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141" s="13"/>
+      <c r="B141" s="13"/>
+      <c r="C141" s="13"/>
+      <c r="D141" s="13"/>
+      <c r="E141" s="13"/>
+      <c r="F141" s="15"/>
+      <c r="G141" s="13"/>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142" s="13"/>
+      <c r="B142" s="13"/>
+      <c r="C142" s="13"/>
+      <c r="D142" s="13"/>
+      <c r="E142" s="13"/>
+      <c r="F142" s="15"/>
+      <c r="G142" s="13"/>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143" s="13"/>
+      <c r="B143" s="13"/>
+      <c r="C143" s="13"/>
+      <c r="D143" s="13"/>
+      <c r="E143" s="13"/>
+      <c r="F143" s="15"/>
+      <c r="G143" s="13"/>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144" s="13"/>
+      <c r="B144" s="13"/>
+      <c r="C144" s="13"/>
+      <c r="D144" s="13"/>
+      <c r="E144" s="13"/>
+      <c r="F144" s="15"/>
+      <c r="G144" s="13"/>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" s="13"/>
+      <c r="B145" s="13"/>
+      <c r="C145" s="13"/>
+      <c r="D145" s="13"/>
+      <c r="E145" s="13"/>
+      <c r="F145" s="15"/>
+      <c r="G145" s="13"/>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146" s="13"/>
+      <c r="B146" s="13"/>
+      <c r="C146" s="13"/>
+      <c r="D146" s="13"/>
+      <c r="E146" s="13"/>
+      <c r="F146" s="15"/>
+      <c r="G146" s="13"/>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147" s="13"/>
+      <c r="B147" s="13"/>
+      <c r="C147" s="13"/>
+      <c r="D147" s="13"/>
+      <c r="E147" s="13"/>
+      <c r="F147" s="15"/>
+      <c r="G147" s="13"/>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148" s="13"/>
+      <c r="B148" s="13"/>
+      <c r="C148" s="13"/>
+      <c r="D148" s="13"/>
+      <c r="E148" s="13"/>
+      <c r="F148" s="15"/>
+      <c r="G148" s="13"/>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149" s="13"/>
+      <c r="B149" s="13"/>
+      <c r="C149" s="13"/>
+      <c r="D149" s="13"/>
+      <c r="E149" s="13"/>
+      <c r="F149" s="15"/>
+      <c r="G149" s="13"/>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A150" s="13"/>
+      <c r="B150" s="13"/>
+      <c r="C150" s="13"/>
+      <c r="D150" s="13"/>
+      <c r="E150" s="13"/>
+      <c r="F150" s="15"/>
+      <c r="G150" s="13"/>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A151" s="13"/>
+      <c r="B151" s="13"/>
+      <c r="C151" s="13"/>
+      <c r="D151" s="13"/>
+      <c r="E151" s="13"/>
+      <c r="F151" s="15"/>
+      <c r="G151" s="13"/>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152" s="13"/>
+      <c r="B152" s="13"/>
+      <c r="C152" s="13"/>
+      <c r="D152" s="13"/>
+      <c r="E152" s="13"/>
+      <c r="F152" s="15"/>
+      <c r="G152" s="13"/>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A153" s="13"/>
+      <c r="B153" s="13"/>
+      <c r="C153" s="13"/>
+      <c r="D153" s="13"/>
+      <c r="E153" s="13"/>
+      <c r="F153" s="15"/>
+      <c r="G153" s="13"/>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A154" s="13"/>
+      <c r="B154" s="13"/>
+      <c r="C154" s="13"/>
+      <c r="D154" s="13"/>
+      <c r="E154" s="13"/>
+      <c r="F154" s="15"/>
+      <c r="G154" s="13"/>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155" s="13"/>
+      <c r="B155" s="13"/>
+      <c r="C155" s="13"/>
+      <c r="D155" s="13"/>
+      <c r="E155" s="13"/>
+      <c r="F155" s="15"/>
+      <c r="G155" s="13"/>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156" s="13"/>
+      <c r="B156" s="13"/>
+      <c r="C156" s="13"/>
+      <c r="D156" s="13"/>
+      <c r="E156" s="13"/>
+      <c r="F156" s="15"/>
+      <c r="G156" s="13"/>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A157" s="13"/>
+      <c r="B157" s="13"/>
+      <c r="C157" s="13"/>
+      <c r="D157" s="13"/>
+      <c r="E157" s="13"/>
+      <c r="F157" s="15"/>
+      <c r="G157" s="13"/>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A158" s="13"/>
+      <c r="B158" s="13"/>
+      <c r="C158" s="13"/>
+      <c r="D158" s="13"/>
+      <c r="E158" s="13"/>
+      <c r="F158" s="15"/>
+      <c r="G158" s="13"/>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A159" s="13"/>
+      <c r="B159" s="13"/>
+      <c r="C159" s="13"/>
+      <c r="D159" s="13"/>
+      <c r="E159" s="13"/>
+      <c r="F159" s="15"/>
+      <c r="G159" s="13"/>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A160" s="13"/>
+      <c r="B160" s="13"/>
+      <c r="C160" s="13"/>
+      <c r="D160" s="13"/>
+      <c r="E160" s="13"/>
+      <c r="F160" s="15"/>
+      <c r="G160" s="13"/>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161" s="13"/>
+      <c r="B161" s="13"/>
+      <c r="C161" s="13"/>
+      <c r="D161" s="13"/>
+      <c r="E161" s="13"/>
+      <c r="F161" s="15"/>
+      <c r="G161" s="13"/>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A162" s="13"/>
+      <c r="B162" s="13"/>
+      <c r="C162" s="13"/>
+      <c r="D162" s="13"/>
+      <c r="E162" s="13"/>
+      <c r="F162" s="15"/>
+      <c r="G162" s="13"/>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A163" s="13"/>
+      <c r="B163" s="13"/>
+      <c r="C163" s="13"/>
+      <c r="D163" s="13"/>
+      <c r="E163" s="13"/>
+      <c r="F163" s="15"/>
+      <c r="G163" s="13"/>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A164" s="13"/>
+      <c r="B164" s="13"/>
+      <c r="C164" s="13"/>
+      <c r="D164" s="13"/>
+      <c r="E164" s="13"/>
+      <c r="F164" s="15"/>
+      <c r="G164" s="13"/>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165" s="13"/>
+      <c r="B165" s="13"/>
+      <c r="C165" s="13"/>
+      <c r="D165" s="13"/>
+      <c r="E165" s="13"/>
+      <c r="F165" s="15"/>
+      <c r="G165" s="13"/>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A166" s="13"/>
+      <c r="B166" s="13"/>
+      <c r="C166" s="13"/>
+      <c r="D166" s="13"/>
+      <c r="E166" s="13"/>
+      <c r="F166" s="15"/>
+      <c r="G166" s="13"/>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A167" s="13"/>
+      <c r="B167" s="13"/>
+      <c r="C167" s="13"/>
+      <c r="D167" s="13"/>
+      <c r="E167" s="13"/>
+      <c r="F167" s="15"/>
+      <c r="G167" s="13"/>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A168" s="13"/>
+      <c r="B168" s="13"/>
+      <c r="C168" s="13"/>
+      <c r="D168" s="13"/>
+      <c r="E168" s="13"/>
+      <c r="F168" s="15"/>
+      <c r="G168" s="13"/>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A169" s="13"/>
+      <c r="B169" s="13"/>
+      <c r="C169" s="13"/>
+      <c r="D169" s="13"/>
+      <c r="E169" s="13"/>
+      <c r="F169" s="15"/>
+      <c r="G169" s="13"/>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A170" s="13"/>
+      <c r="B170" s="13"/>
+      <c r="C170" s="13"/>
+      <c r="D170" s="13"/>
+      <c r="E170" s="13"/>
+      <c r="F170" s="15"/>
+      <c r="G170" s="13"/>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A171" s="13"/>
+      <c r="B171" s="13"/>
+      <c r="C171" s="13"/>
+      <c r="D171" s="13"/>
+      <c r="E171" s="13"/>
+      <c r="F171" s="15"/>
+      <c r="G171" s="13"/>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A172" s="13"/>
+      <c r="B172" s="13"/>
+      <c r="C172" s="13"/>
+      <c r="D172" s="13"/>
+      <c r="E172" s="13"/>
+      <c r="F172" s="15"/>
+      <c r="G172" s="13"/>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A173" s="13"/>
+      <c r="B173" s="13"/>
+      <c r="C173" s="13"/>
+      <c r="D173" s="13"/>
+      <c r="E173" s="13"/>
+      <c r="F173" s="15"/>
+      <c r="G173" s="13"/>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A174" s="13"/>
+      <c r="B174" s="13"/>
+      <c r="C174" s="13"/>
+      <c r="D174" s="13"/>
+      <c r="E174" s="13"/>
+      <c r="F174" s="15"/>
+      <c r="G174" s="13"/>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A175" s="13"/>
+      <c r="B175" s="13"/>
+      <c r="C175" s="13"/>
+      <c r="D175" s="13"/>
+      <c r="E175" s="13"/>
+      <c r="F175" s="15"/>
+      <c r="G175" s="13"/>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A176" s="13"/>
+      <c r="B176" s="13"/>
+      <c r="C176" s="13"/>
+      <c r="D176" s="13"/>
+      <c r="E176" s="13"/>
+      <c r="F176" s="15"/>
+      <c r="G176" s="13"/>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A177" s="13"/>
+      <c r="B177" s="13"/>
+      <c r="C177" s="13"/>
+      <c r="D177" s="13"/>
+      <c r="E177" s="13"/>
+      <c r="F177" s="15"/>
+      <c r="G177" s="13"/>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A178" s="13"/>
+      <c r="B178" s="13"/>
+      <c r="C178" s="13"/>
+      <c r="D178" s="13"/>
+      <c r="E178" s="13"/>
+      <c r="F178" s="15"/>
+      <c r="G178" s="13"/>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A179" s="13"/>
+      <c r="B179" s="13"/>
+      <c r="C179" s="13"/>
+      <c r="D179" s="13"/>
+      <c r="E179" s="13"/>
+      <c r="F179" s="15"/>
+      <c r="G179" s="13"/>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A180" s="13"/>
+      <c r="B180" s="13"/>
+      <c r="C180" s="13"/>
+      <c r="D180" s="13"/>
+      <c r="E180" s="13"/>
+      <c r="F180" s="15"/>
+      <c r="G180" s="13"/>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A181" s="13"/>
+      <c r="B181" s="13"/>
+      <c r="C181" s="13"/>
+      <c r="D181" s="13"/>
+      <c r="E181" s="13"/>
+      <c r="F181" s="15"/>
+      <c r="G181" s="13"/>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A182" s="13"/>
+      <c r="B182" s="13"/>
+      <c r="C182" s="13"/>
+      <c r="D182" s="13"/>
+      <c r="E182" s="13"/>
+      <c r="F182" s="15"/>
+      <c r="G182" s="13"/>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A183" s="13"/>
+      <c r="B183" s="13"/>
+      <c r="C183" s="13"/>
+      <c r="D183" s="13"/>
+      <c r="E183" s="13"/>
+      <c r="F183" s="15"/>
+      <c r="G183" s="13"/>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A184" s="13"/>
+      <c r="B184" s="13"/>
+      <c r="C184" s="13"/>
+      <c r="D184" s="13"/>
+      <c r="E184" s="13"/>
+      <c r="F184" s="15"/>
+      <c r="G184" s="13"/>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A185" s="13"/>
+      <c r="B185" s="13"/>
+      <c r="C185" s="13"/>
+      <c r="D185" s="13"/>
+      <c r="E185" s="13"/>
+      <c r="F185" s="15"/>
+      <c r="G185" s="13"/>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A186" s="13"/>
+      <c r="B186" s="13"/>
+      <c r="C186" s="13"/>
+      <c r="D186" s="13"/>
+      <c r="E186" s="13"/>
+      <c r="F186" s="15"/>
+      <c r="G186" s="13"/>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A187" s="13"/>
+      <c r="B187" s="13"/>
+      <c r="C187" s="13"/>
+      <c r="D187" s="13"/>
+      <c r="E187" s="13"/>
+      <c r="F187" s="15"/>
+      <c r="G187" s="13"/>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A188" s="13"/>
+      <c r="B188" s="13"/>
+      <c r="C188" s="13"/>
+      <c r="D188" s="13"/>
+      <c r="E188" s="13"/>
+      <c r="F188" s="15"/>
+      <c r="G188" s="13"/>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A189" s="13"/>
+      <c r="B189" s="13"/>
+      <c r="C189" s="13"/>
+      <c r="D189" s="13"/>
+      <c r="E189" s="13"/>
+      <c r="F189" s="15"/>
+      <c r="G189" s="13"/>
+    </row>
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A190" s="13"/>
+      <c r="B190" s="13"/>
+      <c r="C190" s="13"/>
+      <c r="D190" s="13"/>
+      <c r="E190" s="13"/>
+      <c r="F190" s="15"/>
+      <c r="G190" s="13"/>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A191" s="13"/>
+      <c r="B191" s="13"/>
+      <c r="C191" s="13"/>
+      <c r="D191" s="13"/>
+      <c r="E191" s="13"/>
+      <c r="F191" s="15"/>
+      <c r="G191" s="13"/>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A192" s="13"/>
+      <c r="B192" s="13"/>
+      <c r="C192" s="13"/>
+      <c r="D192" s="13"/>
+      <c r="E192" s="13"/>
+      <c r="F192" s="15"/>
+      <c r="G192" s="13"/>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A193" s="13"/>
+      <c r="B193" s="13"/>
+      <c r="C193" s="13"/>
+      <c r="D193" s="13"/>
+      <c r="E193" s="13"/>
+      <c r="F193" s="15"/>
+      <c r="G193" s="13"/>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A194" s="13"/>
+      <c r="B194" s="13"/>
+      <c r="C194" s="13"/>
+      <c r="D194" s="13"/>
+      <c r="E194" s="13"/>
+      <c r="F194" s="15"/>
+      <c r="G194" s="13"/>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A195" s="13"/>
+      <c r="B195" s="13"/>
+      <c r="C195" s="13"/>
+      <c r="D195" s="13"/>
+      <c r="E195" s="13"/>
+      <c r="F195" s="15"/>
+      <c r="G195" s="13"/>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A196" s="13"/>
+      <c r="B196" s="13"/>
+      <c r="C196" s="13"/>
+      <c r="D196" s="13"/>
+      <c r="E196" s="13"/>
+      <c r="F196" s="15"/>
+      <c r="G196" s="13"/>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A197" s="13"/>
+      <c r="B197" s="13"/>
+      <c r="C197" s="13"/>
+      <c r="D197" s="13"/>
+      <c r="E197" s="13"/>
+      <c r="F197" s="15"/>
+      <c r="G197" s="13"/>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A198" s="13"/>
+      <c r="B198" s="13"/>
+      <c r="C198" s="13"/>
+      <c r="D198" s="13"/>
+      <c r="E198" s="13"/>
+      <c r="F198" s="15"/>
+      <c r="G198" s="13"/>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A199" s="16"/>
+      <c r="B199" s="16"/>
+      <c r="C199" s="16"/>
+      <c r="D199" s="16"/>
+      <c r="E199" s="16"/>
+      <c r="F199" s="15"/>
+      <c r="G199" s="13"/>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A200" s="13"/>
+      <c r="B200" s="13"/>
+      <c r="C200" s="13"/>
+      <c r="D200" s="13"/>
+      <c r="E200" s="13"/>
+      <c r="F200" s="15"/>
+      <c r="G200" s="13"/>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A201" s="13"/>
+      <c r="B201" s="13"/>
+      <c r="C201" s="13"/>
+      <c r="D201" s="13"/>
+      <c r="E201" s="13"/>
+      <c r="F201" s="17"/>
+      <c r="G201" s="16"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="無効なアセットの型" error="サポートされている型を選択してください。" sqref="E2:E1048576" xr:uid="{DAFCEDAC-664F-4E66-8E89-E25F0B4ECB3E}">
+      <formula1>"Text,Bool,Integer,Credential"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Roles Assignment Model" error="Please select a supported Roles Assignment model." sqref="B202:B1048576" xr:uid="{2BF73C75-D775-4B85-AC28-CE587C33F49C}">
+      <formula1>"Custom Roles,Inherit from tenant"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="無効なアセットのスコープ" error="サポートされているスコープを選択してください。" sqref="C2:C1048576" xr:uid="{85833D7A-7854-4817-A494-26A72E5BAF16}">
+      <formula1>"Global,Robot"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8137958-4AF5-4B95-A694-D874E76F8AD9}">
   <dimension ref="A1:E201"/>
   <sheetViews>
@@ -2769,10 +4702,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>3</v>
@@ -4201,7 +6134,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD1CBAFE-B49D-4BE5-96DE-012190C0FEDD}">
   <dimension ref="A1:D201"/>
   <sheetViews>
@@ -4222,7 +6155,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>3</v>
@@ -5445,7 +7378,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0575E39A-89C3-4F01-996C-47476CE87082}">
   <dimension ref="A1:E201"/>
   <sheetViews>
@@ -5467,10 +7400,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>3</v>
@@ -6894,1454 +8827,4 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D09A84AA-342E-407D-AB3E-4B1D94744C9A}">
-  <dimension ref="A1:E201"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.140625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="45.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="2"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="2"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="2"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="2"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="2"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="2"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="2"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="2"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="2"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="2"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="2"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="2"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="2"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="2"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="2"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="2"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="2"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="2"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="2"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="2"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="2"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="2"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="2"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="2"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="2"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="2"/>
-      <c r="B57" s="2"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="2"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="2"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="2"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="2"/>
-      <c r="B60" s="2"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="2"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="2"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="2"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="2"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="2"/>
-      <c r="B63" s="2"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="2"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="2"/>
-      <c r="B64" s="2"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="2"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="2"/>
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="2"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="2"/>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="2"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="2"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="2"/>
-      <c r="B68" s="2"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="2"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="2"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="2"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="2"/>
-      <c r="B70" s="2"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="2"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" s="2"/>
-      <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="3"/>
-      <c r="E71" s="2"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A72" s="2"/>
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="2"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="2"/>
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="2"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="2"/>
-      <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="2"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="2"/>
-      <c r="B75" s="2"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="2"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="2"/>
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="3"/>
-      <c r="E76" s="2"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="2"/>
-      <c r="B77" s="2"/>
-      <c r="C77" s="2"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="2"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="2"/>
-      <c r="B78" s="2"/>
-      <c r="C78" s="2"/>
-      <c r="D78" s="3"/>
-      <c r="E78" s="2"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="2"/>
-      <c r="B79" s="2"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="3"/>
-      <c r="E79" s="2"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="2"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="3"/>
-      <c r="E80" s="2"/>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="2"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="3"/>
-      <c r="E81" s="2"/>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="2"/>
-      <c r="B82" s="2"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="3"/>
-      <c r="E82" s="2"/>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="2"/>
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
-      <c r="D83" s="3"/>
-      <c r="E83" s="2"/>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="2"/>
-      <c r="B84" s="2"/>
-      <c r="C84" s="2"/>
-      <c r="D84" s="3"/>
-      <c r="E84" s="2"/>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="2"/>
-      <c r="B85" s="2"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="3"/>
-      <c r="E85" s="2"/>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="2"/>
-      <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
-      <c r="D86" s="3"/>
-      <c r="E86" s="2"/>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="2"/>
-      <c r="B87" s="2"/>
-      <c r="C87" s="2"/>
-      <c r="D87" s="3"/>
-      <c r="E87" s="2"/>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="2"/>
-      <c r="B88" s="2"/>
-      <c r="C88" s="2"/>
-      <c r="D88" s="3"/>
-      <c r="E88" s="2"/>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="2"/>
-      <c r="B89" s="2"/>
-      <c r="C89" s="2"/>
-      <c r="D89" s="3"/>
-      <c r="E89" s="2"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="2"/>
-      <c r="B90" s="2"/>
-      <c r="C90" s="2"/>
-      <c r="D90" s="3"/>
-      <c r="E90" s="2"/>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="2"/>
-      <c r="B91" s="2"/>
-      <c r="C91" s="2"/>
-      <c r="D91" s="3"/>
-      <c r="E91" s="2"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="2"/>
-      <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
-      <c r="D92" s="3"/>
-      <c r="E92" s="2"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="2"/>
-      <c r="B93" s="2"/>
-      <c r="C93" s="2"/>
-      <c r="D93" s="3"/>
-      <c r="E93" s="2"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A94" s="2"/>
-      <c r="B94" s="2"/>
-      <c r="C94" s="2"/>
-      <c r="D94" s="3"/>
-      <c r="E94" s="2"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A95" s="2"/>
-      <c r="B95" s="2"/>
-      <c r="C95" s="2"/>
-      <c r="D95" s="3"/>
-      <c r="E95" s="2"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A96" s="2"/>
-      <c r="B96" s="2"/>
-      <c r="C96" s="2"/>
-      <c r="D96" s="3"/>
-      <c r="E96" s="2"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="2"/>
-      <c r="B97" s="2"/>
-      <c r="C97" s="2"/>
-      <c r="D97" s="3"/>
-      <c r="E97" s="2"/>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="2"/>
-      <c r="B98" s="2"/>
-      <c r="C98" s="2"/>
-      <c r="D98" s="3"/>
-      <c r="E98" s="2"/>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="2"/>
-      <c r="B99" s="2"/>
-      <c r="C99" s="2"/>
-      <c r="D99" s="3"/>
-      <c r="E99" s="2"/>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A100" s="2"/>
-      <c r="B100" s="2"/>
-      <c r="C100" s="2"/>
-      <c r="D100" s="3"/>
-      <c r="E100" s="2"/>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A101" s="2"/>
-      <c r="B101" s="2"/>
-      <c r="C101" s="2"/>
-      <c r="D101" s="3"/>
-      <c r="E101" s="2"/>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A102" s="2"/>
-      <c r="B102" s="2"/>
-      <c r="C102" s="2"/>
-      <c r="D102" s="3"/>
-      <c r="E102" s="2"/>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A103" s="2"/>
-      <c r="B103" s="2"/>
-      <c r="C103" s="2"/>
-      <c r="D103" s="3"/>
-      <c r="E103" s="2"/>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" s="2"/>
-      <c r="B104" s="2"/>
-      <c r="C104" s="2"/>
-      <c r="D104" s="3"/>
-      <c r="E104" s="2"/>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A105" s="2"/>
-      <c r="B105" s="2"/>
-      <c r="C105" s="2"/>
-      <c r="D105" s="3"/>
-      <c r="E105" s="2"/>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A106" s="2"/>
-      <c r="B106" s="2"/>
-      <c r="C106" s="2"/>
-      <c r="D106" s="3"/>
-      <c r="E106" s="2"/>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="2"/>
-      <c r="B107" s="2"/>
-      <c r="C107" s="2"/>
-      <c r="D107" s="3"/>
-      <c r="E107" s="2"/>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A108" s="2"/>
-      <c r="B108" s="2"/>
-      <c r="C108" s="2"/>
-      <c r="D108" s="3"/>
-      <c r="E108" s="2"/>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" s="2"/>
-      <c r="B109" s="2"/>
-      <c r="C109" s="2"/>
-      <c r="D109" s="3"/>
-      <c r="E109" s="2"/>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A110" s="2"/>
-      <c r="B110" s="2"/>
-      <c r="C110" s="2"/>
-      <c r="D110" s="3"/>
-      <c r="E110" s="2"/>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A111" s="2"/>
-      <c r="B111" s="2"/>
-      <c r="C111" s="2"/>
-      <c r="D111" s="3"/>
-      <c r="E111" s="2"/>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A112" s="2"/>
-      <c r="B112" s="2"/>
-      <c r="C112" s="2"/>
-      <c r="D112" s="3"/>
-      <c r="E112" s="2"/>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" s="2"/>
-      <c r="B113" s="2"/>
-      <c r="C113" s="2"/>
-      <c r="D113" s="3"/>
-      <c r="E113" s="2"/>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="2"/>
-      <c r="B114" s="2"/>
-      <c r="C114" s="2"/>
-      <c r="D114" s="3"/>
-      <c r="E114" s="2"/>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" s="2"/>
-      <c r="B115" s="2"/>
-      <c r="C115" s="2"/>
-      <c r="D115" s="3"/>
-      <c r="E115" s="2"/>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A116" s="2"/>
-      <c r="B116" s="2"/>
-      <c r="C116" s="2"/>
-      <c r="D116" s="3"/>
-      <c r="E116" s="2"/>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" s="2"/>
-      <c r="B117" s="2"/>
-      <c r="C117" s="2"/>
-      <c r="D117" s="3"/>
-      <c r="E117" s="2"/>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A118" s="2"/>
-      <c r="B118" s="2"/>
-      <c r="C118" s="2"/>
-      <c r="D118" s="3"/>
-      <c r="E118" s="2"/>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A119" s="2"/>
-      <c r="B119" s="2"/>
-      <c r="C119" s="2"/>
-      <c r="D119" s="3"/>
-      <c r="E119" s="2"/>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A120" s="2"/>
-      <c r="B120" s="2"/>
-      <c r="C120" s="2"/>
-      <c r="D120" s="3"/>
-      <c r="E120" s="2"/>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121" s="2"/>
-      <c r="B121" s="2"/>
-      <c r="C121" s="2"/>
-      <c r="D121" s="3"/>
-      <c r="E121" s="2"/>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122" s="2"/>
-      <c r="B122" s="2"/>
-      <c r="C122" s="2"/>
-      <c r="D122" s="3"/>
-      <c r="E122" s="2"/>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123" s="2"/>
-      <c r="B123" s="2"/>
-      <c r="C123" s="2"/>
-      <c r="D123" s="3"/>
-      <c r="E123" s="2"/>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" s="2"/>
-      <c r="B124" s="2"/>
-      <c r="C124" s="2"/>
-      <c r="D124" s="3"/>
-      <c r="E124" s="2"/>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125" s="2"/>
-      <c r="B125" s="2"/>
-      <c r="C125" s="2"/>
-      <c r="D125" s="3"/>
-      <c r="E125" s="2"/>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A126" s="2"/>
-      <c r="B126" s="2"/>
-      <c r="C126" s="2"/>
-      <c r="D126" s="3"/>
-      <c r="E126" s="2"/>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A127" s="2"/>
-      <c r="B127" s="2"/>
-      <c r="C127" s="2"/>
-      <c r="D127" s="3"/>
-      <c r="E127" s="2"/>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A128" s="2"/>
-      <c r="B128" s="2"/>
-      <c r="C128" s="2"/>
-      <c r="D128" s="3"/>
-      <c r="E128" s="2"/>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A129" s="2"/>
-      <c r="B129" s="2"/>
-      <c r="C129" s="2"/>
-      <c r="D129" s="3"/>
-      <c r="E129" s="2"/>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A130" s="2"/>
-      <c r="B130" s="2"/>
-      <c r="C130" s="2"/>
-      <c r="D130" s="3"/>
-      <c r="E130" s="2"/>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A131" s="2"/>
-      <c r="B131" s="2"/>
-      <c r="C131" s="2"/>
-      <c r="D131" s="3"/>
-      <c r="E131" s="2"/>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A132" s="2"/>
-      <c r="B132" s="2"/>
-      <c r="C132" s="2"/>
-      <c r="D132" s="3"/>
-      <c r="E132" s="2"/>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A133" s="2"/>
-      <c r="B133" s="2"/>
-      <c r="C133" s="2"/>
-      <c r="D133" s="3"/>
-      <c r="E133" s="2"/>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A134" s="2"/>
-      <c r="B134" s="2"/>
-      <c r="C134" s="2"/>
-      <c r="D134" s="3"/>
-      <c r="E134" s="2"/>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A135" s="2"/>
-      <c r="B135" s="2"/>
-      <c r="C135" s="2"/>
-      <c r="D135" s="3"/>
-      <c r="E135" s="2"/>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A136" s="2"/>
-      <c r="B136" s="2"/>
-      <c r="C136" s="2"/>
-      <c r="D136" s="3"/>
-      <c r="E136" s="2"/>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A137" s="2"/>
-      <c r="B137" s="2"/>
-      <c r="C137" s="2"/>
-      <c r="D137" s="3"/>
-      <c r="E137" s="2"/>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A138" s="2"/>
-      <c r="B138" s="2"/>
-      <c r="C138" s="2"/>
-      <c r="D138" s="3"/>
-      <c r="E138" s="2"/>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A139" s="2"/>
-      <c r="B139" s="2"/>
-      <c r="C139" s="2"/>
-      <c r="D139" s="3"/>
-      <c r="E139" s="2"/>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A140" s="2"/>
-      <c r="B140" s="2"/>
-      <c r="C140" s="2"/>
-      <c r="D140" s="3"/>
-      <c r="E140" s="2"/>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A141" s="2"/>
-      <c r="B141" s="2"/>
-      <c r="C141" s="2"/>
-      <c r="D141" s="3"/>
-      <c r="E141" s="2"/>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A142" s="2"/>
-      <c r="B142" s="2"/>
-      <c r="C142" s="2"/>
-      <c r="D142" s="3"/>
-      <c r="E142" s="2"/>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A143" s="2"/>
-      <c r="B143" s="2"/>
-      <c r="C143" s="2"/>
-      <c r="D143" s="3"/>
-      <c r="E143" s="2"/>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A144" s="2"/>
-      <c r="B144" s="2"/>
-      <c r="C144" s="2"/>
-      <c r="D144" s="3"/>
-      <c r="E144" s="2"/>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A145" s="2"/>
-      <c r="B145" s="2"/>
-      <c r="C145" s="2"/>
-      <c r="D145" s="3"/>
-      <c r="E145" s="2"/>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A146" s="2"/>
-      <c r="B146" s="2"/>
-      <c r="C146" s="2"/>
-      <c r="D146" s="3"/>
-      <c r="E146" s="2"/>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A147" s="2"/>
-      <c r="B147" s="2"/>
-      <c r="C147" s="2"/>
-      <c r="D147" s="3"/>
-      <c r="E147" s="2"/>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A148" s="2"/>
-      <c r="B148" s="2"/>
-      <c r="C148" s="2"/>
-      <c r="D148" s="3"/>
-      <c r="E148" s="2"/>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A149" s="2"/>
-      <c r="B149" s="2"/>
-      <c r="C149" s="2"/>
-      <c r="D149" s="3"/>
-      <c r="E149" s="2"/>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A150" s="2"/>
-      <c r="B150" s="2"/>
-      <c r="C150" s="2"/>
-      <c r="D150" s="3"/>
-      <c r="E150" s="2"/>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A151" s="2"/>
-      <c r="B151" s="2"/>
-      <c r="C151" s="2"/>
-      <c r="D151" s="3"/>
-      <c r="E151" s="2"/>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A152" s="2"/>
-      <c r="B152" s="2"/>
-      <c r="C152" s="2"/>
-      <c r="D152" s="3"/>
-      <c r="E152" s="2"/>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A153" s="2"/>
-      <c r="B153" s="2"/>
-      <c r="C153" s="2"/>
-      <c r="D153" s="3"/>
-      <c r="E153" s="2"/>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A154" s="2"/>
-      <c r="B154" s="2"/>
-      <c r="C154" s="2"/>
-      <c r="D154" s="3"/>
-      <c r="E154" s="2"/>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A155" s="2"/>
-      <c r="B155" s="2"/>
-      <c r="C155" s="2"/>
-      <c r="D155" s="3"/>
-      <c r="E155" s="2"/>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A156" s="2"/>
-      <c r="B156" s="2"/>
-      <c r="C156" s="2"/>
-      <c r="D156" s="3"/>
-      <c r="E156" s="2"/>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A157" s="2"/>
-      <c r="B157" s="2"/>
-      <c r="C157" s="2"/>
-      <c r="D157" s="3"/>
-      <c r="E157" s="2"/>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A158" s="2"/>
-      <c r="B158" s="2"/>
-      <c r="C158" s="2"/>
-      <c r="D158" s="3"/>
-      <c r="E158" s="2"/>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A159" s="2"/>
-      <c r="B159" s="2"/>
-      <c r="C159" s="2"/>
-      <c r="D159" s="3"/>
-      <c r="E159" s="2"/>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A160" s="2"/>
-      <c r="B160" s="2"/>
-      <c r="C160" s="2"/>
-      <c r="D160" s="3"/>
-      <c r="E160" s="2"/>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A161" s="2"/>
-      <c r="B161" s="2"/>
-      <c r="C161" s="2"/>
-      <c r="D161" s="3"/>
-      <c r="E161" s="2"/>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A162" s="2"/>
-      <c r="B162" s="2"/>
-      <c r="C162" s="2"/>
-      <c r="D162" s="3"/>
-      <c r="E162" s="2"/>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A163" s="2"/>
-      <c r="B163" s="2"/>
-      <c r="C163" s="2"/>
-      <c r="D163" s="3"/>
-      <c r="E163" s="2"/>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A164" s="2"/>
-      <c r="B164" s="2"/>
-      <c r="C164" s="2"/>
-      <c r="D164" s="3"/>
-      <c r="E164" s="2"/>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A165" s="2"/>
-      <c r="B165" s="2"/>
-      <c r="C165" s="2"/>
-      <c r="D165" s="3"/>
-      <c r="E165" s="2"/>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A166" s="2"/>
-      <c r="B166" s="2"/>
-      <c r="C166" s="2"/>
-      <c r="D166" s="3"/>
-      <c r="E166" s="2"/>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A167" s="2"/>
-      <c r="B167" s="2"/>
-      <c r="C167" s="2"/>
-      <c r="D167" s="3"/>
-      <c r="E167" s="2"/>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A168" s="2"/>
-      <c r="B168" s="2"/>
-      <c r="C168" s="2"/>
-      <c r="D168" s="3"/>
-      <c r="E168" s="2"/>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A169" s="2"/>
-      <c r="B169" s="2"/>
-      <c r="C169" s="2"/>
-      <c r="D169" s="3"/>
-      <c r="E169" s="2"/>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A170" s="2"/>
-      <c r="B170" s="2"/>
-      <c r="C170" s="2"/>
-      <c r="D170" s="3"/>
-      <c r="E170" s="2"/>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A171" s="2"/>
-      <c r="B171" s="2"/>
-      <c r="C171" s="2"/>
-      <c r="D171" s="3"/>
-      <c r="E171" s="2"/>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A172" s="2"/>
-      <c r="B172" s="2"/>
-      <c r="C172" s="2"/>
-      <c r="D172" s="3"/>
-      <c r="E172" s="2"/>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A173" s="2"/>
-      <c r="B173" s="2"/>
-      <c r="C173" s="2"/>
-      <c r="D173" s="3"/>
-      <c r="E173" s="2"/>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A174" s="2"/>
-      <c r="B174" s="2"/>
-      <c r="C174" s="2"/>
-      <c r="D174" s="3"/>
-      <c r="E174" s="2"/>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A175" s="2"/>
-      <c r="B175" s="2"/>
-      <c r="C175" s="2"/>
-      <c r="D175" s="3"/>
-      <c r="E175" s="2"/>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A176" s="2"/>
-      <c r="B176" s="2"/>
-      <c r="C176" s="2"/>
-      <c r="D176" s="3"/>
-      <c r="E176" s="2"/>
-    </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A177" s="2"/>
-      <c r="B177" s="2"/>
-      <c r="C177" s="2"/>
-      <c r="D177" s="3"/>
-      <c r="E177" s="2"/>
-    </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A178" s="2"/>
-      <c r="B178" s="2"/>
-      <c r="C178" s="2"/>
-      <c r="D178" s="3"/>
-      <c r="E178" s="2"/>
-    </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A179" s="2"/>
-      <c r="B179" s="2"/>
-      <c r="C179" s="2"/>
-      <c r="D179" s="3"/>
-      <c r="E179" s="2"/>
-    </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A180" s="2"/>
-      <c r="B180" s="2"/>
-      <c r="C180" s="2"/>
-      <c r="D180" s="3"/>
-      <c r="E180" s="2"/>
-    </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A181" s="2"/>
-      <c r="B181" s="2"/>
-      <c r="C181" s="2"/>
-      <c r="D181" s="3"/>
-      <c r="E181" s="2"/>
-    </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A182" s="2"/>
-      <c r="B182" s="2"/>
-      <c r="C182" s="2"/>
-      <c r="D182" s="3"/>
-      <c r="E182" s="2"/>
-    </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A183" s="2"/>
-      <c r="B183" s="2"/>
-      <c r="C183" s="2"/>
-      <c r="D183" s="3"/>
-      <c r="E183" s="2"/>
-    </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A184" s="2"/>
-      <c r="B184" s="2"/>
-      <c r="C184" s="2"/>
-      <c r="D184" s="3"/>
-      <c r="E184" s="2"/>
-    </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A185" s="2"/>
-      <c r="B185" s="2"/>
-      <c r="C185" s="2"/>
-      <c r="D185" s="3"/>
-      <c r="E185" s="2"/>
-    </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A186" s="2"/>
-      <c r="B186" s="2"/>
-      <c r="C186" s="2"/>
-      <c r="D186" s="3"/>
-      <c r="E186" s="2"/>
-    </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A187" s="2"/>
-      <c r="B187" s="2"/>
-      <c r="C187" s="2"/>
-      <c r="D187" s="3"/>
-      <c r="E187" s="2"/>
-    </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A188" s="2"/>
-      <c r="B188" s="2"/>
-      <c r="C188" s="2"/>
-      <c r="D188" s="3"/>
-      <c r="E188" s="2"/>
-    </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A189" s="2"/>
-      <c r="B189" s="2"/>
-      <c r="C189" s="2"/>
-      <c r="D189" s="3"/>
-      <c r="E189" s="2"/>
-    </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A190" s="2"/>
-      <c r="B190" s="2"/>
-      <c r="C190" s="2"/>
-      <c r="D190" s="3"/>
-      <c r="E190" s="2"/>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A191" s="2"/>
-      <c r="B191" s="2"/>
-      <c r="C191" s="2"/>
-      <c r="D191" s="3"/>
-      <c r="E191" s="2"/>
-    </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A192" s="2"/>
-      <c r="B192" s="2"/>
-      <c r="C192" s="2"/>
-      <c r="D192" s="3"/>
-      <c r="E192" s="2"/>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A193" s="2"/>
-      <c r="B193" s="2"/>
-      <c r="C193" s="2"/>
-      <c r="D193" s="3"/>
-      <c r="E193" s="2"/>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A194" s="2"/>
-      <c r="B194" s="2"/>
-      <c r="C194" s="2"/>
-      <c r="D194" s="3"/>
-      <c r="E194" s="2"/>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A195" s="2"/>
-      <c r="B195" s="2"/>
-      <c r="C195" s="2"/>
-      <c r="D195" s="3"/>
-      <c r="E195" s="2"/>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A196" s="2"/>
-      <c r="B196" s="2"/>
-      <c r="C196" s="2"/>
-      <c r="D196" s="3"/>
-      <c r="E196" s="2"/>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A197" s="2"/>
-      <c r="B197" s="2"/>
-      <c r="C197" s="2"/>
-      <c r="D197" s="3"/>
-      <c r="E197" s="2"/>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A198" s="2"/>
-      <c r="B198" s="2"/>
-      <c r="C198" s="2"/>
-      <c r="D198" s="3"/>
-      <c r="E198" s="2"/>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A199" s="6"/>
-      <c r="B199" s="6"/>
-      <c r="C199" s="6"/>
-      <c r="D199" s="3"/>
-      <c r="E199" s="2"/>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A200" s="2"/>
-      <c r="B200" s="2"/>
-      <c r="C200" s="2"/>
-      <c r="D200" s="3"/>
-      <c r="E200" s="2"/>
-    </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A201" s="2"/>
-      <c r="B201" s="2"/>
-      <c r="C201" s="2"/>
-      <c r="D201" s="10"/>
-      <c r="E201" s="6"/>
-    </row>
-  </sheetData>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Roles Assignment Model" error="Please select a supported Roles Assignment model." sqref="B202:B1048576" xr:uid="{6C21B57F-70E6-4DCB-9248-04EEEEA21B49}">
-      <formula1>"Custom Roles,Inherit from tenant"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576" xr:uid="{33323D49-BA9E-4398-8435-DE79F3E9E8F1}">
-      <formula1>"Text,Bool,Integer,Credential"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>